<commit_message>
add lua code generator,and modify some code
</commit_message>
<xml_diff>
--- a/ExcelTool/bin/table/细菌大战数据.xlsx
+++ b/ExcelTool/bin/table/细菌大战数据.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21126"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21DF06C9-225C-49AD-9328-3E75A64BF27E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{860D146C-63CF-42F5-9468-C4FD407708C1}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="228" windowWidth="14808" windowHeight="7896" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="228" windowWidth="14808" windowHeight="7896" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EnviromentGermSetting" sheetId="1" r:id="rId1"/>
@@ -231,7 +231,7 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>对于KVT表，要求第二个字段必须为Value，第三个字段必须为KeyDes</t>
+    <t>对于KVT表，要求第一个字段必须为Key，且是string类型。第二个字段必须为Value，第三个字段必须为KeyDes</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -1015,7 +1015,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88515294-FE01-4CB5-A999-E01A3130B381}">
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -1127,8 +1127,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E35B117-A9CD-4E5C-BF9C-AC94340ED648}">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
xlsx to lua string format
</commit_message>
<xml_diff>
--- a/ExcelTool/bin/table/细菌大战数据.xlsx
+++ b/ExcelTool/bin/table/细菌大战数据.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21126"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{860D146C-63CF-42F5-9468-C4FD407708C1}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8B2AC7B-4B6D-4338-BD64-D77EEF4B5364}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="228" windowWidth="14808" windowHeight="7896" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="228" windowWidth="14808" windowHeight="7896" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EnviromentGermSetting" sheetId="1" r:id="rId1"/>
@@ -151,10 +151,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>阵营:{0}</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>Id</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -163,10 +159,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>分支数:{0}/{1}</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>自己</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -191,14 +183,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>细胞数:{0}/{1}</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>已占领:{0}/{1}</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>BridgeShootCellMinDuration</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -232,6 +216,22 @@
   </si>
   <si>
     <t>对于KVT表，要求第一个字段必须为Key，且是string类型。第二个字段必须为Value，第三个字段必须为KeyDes</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>阵营:s%</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>细胞数:s%}/s%</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>已占领:s%/s%</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>分支数:s%/s%</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -897,7 +897,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>13</v>
@@ -1015,8 +1015,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88515294-FE01-4CB5-A999-E01A3130B381}">
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
@@ -1027,13 +1027,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B1" t="s">
         <v>23</v>
       </c>
       <c r="C1" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -1046,10 +1046,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -1057,7 +1057,7 @@
         <v>1000</v>
       </c>
       <c r="B6" t="s">
-        <v>33</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -1065,7 +1065,7 @@
         <v>1001</v>
       </c>
       <c r="B7" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -1073,7 +1073,7 @@
         <v>1002</v>
       </c>
       <c r="B8" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -1081,7 +1081,7 @@
         <v>1003</v>
       </c>
       <c r="B9" t="s">
-        <v>36</v>
+        <v>53</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -1089,7 +1089,7 @@
         <v>1004</v>
       </c>
       <c r="B10" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -1097,7 +1097,7 @@
         <v>1005</v>
       </c>
       <c r="B11" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -1105,7 +1105,7 @@
         <v>1006</v>
       </c>
       <c r="B12" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -1113,7 +1113,7 @@
         <v>1007</v>
       </c>
       <c r="B13" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -1127,7 +1127,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E35B117-A9CD-4E5C-BF9C-AC94340ED648}">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
@@ -1147,10 +1147,10 @@
         <v>23</v>
       </c>
       <c r="C1" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="D1" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -1161,15 +1161,15 @@
         <v>16</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C3" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D3" s="11"/>
     </row>
@@ -1215,24 +1215,24 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B9">
         <v>600</v>
       </c>
       <c r="C9" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B10">
         <v>6</v>
       </c>
       <c r="C10" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>